<commit_message>
Added Constituencies to graph
</commit_message>
<xml_diff>
--- a/supports/Constituency.xlsx
+++ b/supports/Constituency.xlsx
@@ -24,135 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
-  <si>
-    <t>Clare</t>
-  </si>
-  <si>
-    <t>Cork East</t>
-  </si>
-  <si>
-    <t>Cork North–Central</t>
-  </si>
-  <si>
-    <t>Cork North–West</t>
-  </si>
-  <si>
-    <t>Cork South–Central</t>
-  </si>
-  <si>
-    <t>Cork South–West</t>
-  </si>
-  <si>
-    <t>Donegal</t>
-  </si>
-  <si>
-    <t>Dublin Bay North</t>
-  </si>
-  <si>
-    <t>Dublin Bay South</t>
-  </si>
-  <si>
-    <t>Dublin Central</t>
-  </si>
-  <si>
-    <t>Dublin Fingal</t>
-  </si>
-  <si>
-    <t>Dublin Mid–West</t>
-  </si>
-  <si>
-    <t>Dublin North–West</t>
-  </si>
-  <si>
-    <t>Dublin Rathdown</t>
-  </si>
-  <si>
-    <t>Dublin South–Central</t>
-  </si>
-  <si>
-    <t>Dublin South–West</t>
-  </si>
-  <si>
-    <t>Dublin West</t>
-  </si>
-  <si>
-    <t>Dún Laoghaire</t>
-  </si>
-  <si>
-    <t>Galway East</t>
-  </si>
-  <si>
-    <t>Galway West</t>
-  </si>
-  <si>
-    <t>Kerry</t>
-  </si>
-  <si>
-    <t>Kildare North</t>
-  </si>
-  <si>
-    <t>Kildare South</t>
-  </si>
-  <si>
-    <t>Laois</t>
-  </si>
-  <si>
-    <t>Limerick City</t>
-  </si>
-  <si>
-    <t>Limerick County</t>
-  </si>
-  <si>
-    <t>Longford–Westmeath</t>
-  </si>
-  <si>
-    <t>Louth</t>
-  </si>
-  <si>
-    <t>Mayo</t>
-  </si>
-  <si>
-    <t>Meath East</t>
-  </si>
-  <si>
-    <t>Meath West</t>
-  </si>
-  <si>
-    <t>Offaly</t>
-  </si>
-  <si>
-    <t>Roscommon–Galway</t>
-  </si>
-  <si>
-    <t>Sligo–Leitrim</t>
-  </si>
-  <si>
-    <t>Tipperary</t>
-  </si>
-  <si>
-    <t>Waterford</t>
-  </si>
-  <si>
-    <t>Wexford</t>
-  </si>
-  <si>
-    <t>Wicklow</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>CREATE</t>
   </si>
   <si>
-    <t>(Carlow–Kilkenny: Constituency</t>
-  </si>
-  <si>
     <t xml:space="preserve">{Population: " 145659", </t>
-  </si>
-  <si>
-    <t>Seats: "5"})</t>
-  </si>
-  <si>
-    <t>CavanMonaghan</t>
   </si>
   <si>
     <t>{Population: "111336",</t>
@@ -268,6 +145,147 @@
   </si>
   <si>
     <t>{Population: "85550",</t>
+  </si>
+  <si>
+    <t>{Population: "87640",</t>
+  </si>
+  <si>
+    <t>{Population: "84586",</t>
+  </si>
+  <si>
+    <t>{Population: "119153",</t>
+  </si>
+  <si>
+    <t>{Population: "147801",</t>
+  </si>
+  <si>
+    <t>{Population: "113795",</t>
+  </si>
+  <si>
+    <t>{Population: "145320",</t>
+  </si>
+  <si>
+    <t>{Population: "141012",</t>
+  </si>
+  <si>
+    <t>Seats:"5"});</t>
+  </si>
+  <si>
+    <t>(CavanMonaghan: Constituency</t>
+  </si>
+  <si>
+    <t>(Clare: Constituency</t>
+  </si>
+  <si>
+    <t>(Cork East: Constituency</t>
+  </si>
+  <si>
+    <t>(Cork NorthCentral: Constituency</t>
+  </si>
+  <si>
+    <t>(Cork NorthWest: Constituency</t>
+  </si>
+  <si>
+    <t>(Cork SouthCentral: Constituency</t>
+  </si>
+  <si>
+    <t>(Cork SouthWest: Constituency</t>
+  </si>
+  <si>
+    <t>(Donegal: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin Bay North: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin Bay South: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin Central: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin Fingal: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin MidWest: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin NorthWest: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin Rathdown: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin SouthCentral: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin SouthWest: Constituency</t>
+  </si>
+  <si>
+    <t>(Dublin West: Constituency</t>
+  </si>
+  <si>
+    <t>(Dún Laoghaire: Constituency</t>
+  </si>
+  <si>
+    <t>(Galway East: Constituency</t>
+  </si>
+  <si>
+    <t>(Galway West: Constituency</t>
+  </si>
+  <si>
+    <t>(Kerry: Constituency</t>
+  </si>
+  <si>
+    <t>(Kildare North: Constituency</t>
+  </si>
+  <si>
+    <t>(Kildare South: Constituency</t>
+  </si>
+  <si>
+    <t>(Laois: Constituency</t>
+  </si>
+  <si>
+    <t>(Limerick City: Constituency</t>
+  </si>
+  <si>
+    <t>(Limerick County: Constituency</t>
+  </si>
+  <si>
+    <t>(LongfordWestmeath: Constituency</t>
+  </si>
+  <si>
+    <t>(Louth: Constituency</t>
+  </si>
+  <si>
+    <t>(Mayo: Constituency</t>
+  </si>
+  <si>
+    <t>(Meath East: Constituency</t>
+  </si>
+  <si>
+    <t>(Meath West: Constituency</t>
+  </si>
+  <si>
+    <t>(Offaly: Constituency</t>
+  </si>
+  <si>
+    <t>(RoscommonGalway: Constituency</t>
+  </si>
+  <si>
+    <t>(SligoLeitrim: Constituency</t>
+  </si>
+  <si>
+    <t>(Tipperary: Constituency</t>
+  </si>
+  <si>
+    <t>(Waterford: Constituency</t>
+  </si>
+  <si>
+    <t>(Wexford: Constituency</t>
+  </si>
+  <si>
+    <t>(Wicklow: Constituency</t>
   </si>
 </sst>
 </file>
@@ -594,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,447 +627,436 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="1">
-        <v>87640</v>
-      </c>
-      <c r="D35">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="1">
-        <v>84586</v>
-      </c>
-      <c r="D36">
-        <v>3</v>
+        <v>78</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="1">
-        <v>119153</v>
-      </c>
-      <c r="D37">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="1">
-        <v>147801</v>
-      </c>
-      <c r="D38">
+        <v>80</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="1">
-        <v>113795</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
+        <v>81</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="1">
-        <v>145320</v>
-      </c>
-      <c r="D40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="1">
-        <v>141012</v>
-      </c>
-      <c r="D41">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the excel spreadsheet and the Constituencies nodes in the graph
</commit_message>
<xml_diff>
--- a/supports/Constituency.xlsx
+++ b/supports/Constituency.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>CREATE</t>
   </si>
   <si>
-    <t xml:space="preserve">{Population: " 145659", </t>
-  </si>
-  <si>
     <t>{Population: "111336",</t>
   </si>
   <si>
@@ -41,15 +38,9 @@
     <t>{Population: "117170",</t>
   </si>
   <si>
-    <t>Seats:"4"}),</t>
-  </si>
-  <si>
     <t>{Population: "86593",</t>
   </si>
   <si>
-    <t>Seats:"3"}),</t>
-  </si>
-  <si>
     <t>{Population: "117952",</t>
   </si>
   <si>
@@ -59,13 +50,7 @@
     <t>{Population: "152358",</t>
   </si>
   <si>
-    <t>Seats:"5"}),</t>
-  </si>
-  <si>
     <t>{Population: "146512",</t>
-  </si>
-  <si>
-    <t>Seats: "5"}),</t>
   </si>
   <si>
     <t>{Population: "116396",</t>
@@ -168,124 +153,247 @@
     <t>{Population: "141012",</t>
   </si>
   <si>
-    <t>Seats:"5"});</t>
-  </si>
-  <si>
-    <t>(CavanMonaghan: Constituency</t>
-  </si>
-  <si>
-    <t>(Clare: Constituency</t>
-  </si>
-  <si>
-    <t>(Cork East: Constituency</t>
-  </si>
-  <si>
-    <t>(Cork NorthCentral: Constituency</t>
-  </si>
-  <si>
-    <t>(Cork NorthWest: Constituency</t>
-  </si>
-  <si>
-    <t>(Cork SouthCentral: Constituency</t>
-  </si>
-  <si>
-    <t>(Cork SouthWest: Constituency</t>
-  </si>
-  <si>
-    <t>(Donegal: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin Bay North: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin Bay South: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin Central: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin Fingal: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin MidWest: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin NorthWest: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin Rathdown: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin SouthCentral: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin SouthWest: Constituency</t>
-  </si>
-  <si>
-    <t>(Dublin West: Constituency</t>
-  </si>
-  <si>
-    <t>(Dún Laoghaire: Constituency</t>
-  </si>
-  <si>
-    <t>(Galway East: Constituency</t>
-  </si>
-  <si>
-    <t>(Galway West: Constituency</t>
-  </si>
-  <si>
     <t>(Kerry: Constituency</t>
   </si>
   <si>
-    <t>(Kildare North: Constituency</t>
-  </si>
-  <si>
-    <t>(Kildare South: Constituency</t>
-  </si>
-  <si>
     <t>(Laois: Constituency</t>
   </si>
   <si>
-    <t>(Limerick City: Constituency</t>
-  </si>
-  <si>
-    <t>(Limerick County: Constituency</t>
-  </si>
-  <si>
-    <t>(LongfordWestmeath: Constituency</t>
-  </si>
-  <si>
     <t>(Louth: Constituency</t>
   </si>
   <si>
     <t>(Mayo: Constituency</t>
   </si>
   <si>
-    <t>(Meath East: Constituency</t>
-  </si>
-  <si>
-    <t>(Meath West: Constituency</t>
-  </si>
-  <si>
-    <t>(Offaly: Constituency</t>
-  </si>
-  <si>
-    <t>(RoscommonGalway: Constituency</t>
-  </si>
-  <si>
-    <t>(SligoLeitrim: Constituency</t>
-  </si>
-  <si>
-    <t>(Tipperary: Constituency</t>
-  </si>
-  <si>
-    <t>(Waterford: Constituency</t>
-  </si>
-  <si>
-    <t>(Wexford: Constituency</t>
-  </si>
-  <si>
-    <t>(Wicklow: Constituency</t>
+    <t>(CM: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "GalwayWest"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Cavan-Monaghan"}),</t>
+  </si>
+  <si>
+    <t>(CE: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Clare"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Cork East"}),</t>
+  </si>
+  <si>
+    <t>(CNC: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Cork North Central"}),</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Cork NorthWest"}),</t>
+  </si>
+  <si>
+    <t>(CNW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Cork SouthCentral"}),</t>
+  </si>
+  <si>
+    <t>(CSC: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Cork SouthWest"}),</t>
+  </si>
+  <si>
+    <t>(CSW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Donegal"}),</t>
+  </si>
+  <si>
+    <t>(DL: Constituency</t>
+  </si>
+  <si>
+    <t>Seats: "5", Name: "Dublin Bay North"}),</t>
+  </si>
+  <si>
+    <t>(DBN: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Dublin Bay South"}),</t>
+  </si>
+  <si>
+    <t>(DBS: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Dublin Central"}),</t>
+  </si>
+  <si>
+    <t>(DC: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Dublin Fingal"}),</t>
+  </si>
+  <si>
+    <t>(DF: Constituency</t>
+  </si>
+  <si>
+    <t>(DMW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Dublin MidWest"}),</t>
+  </si>
+  <si>
+    <t>(DNW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Dublin NorthWest"}),</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Dublin Rathdown"}),</t>
+  </si>
+  <si>
+    <t>(DR: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Dublin SouthCentral"}),</t>
+  </si>
+  <si>
+    <t>(DSC: Constituency</t>
+  </si>
+  <si>
+    <t>(DSW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Dublin SouthWest"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Dublin West"}),</t>
+  </si>
+  <si>
+    <t>(DW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Dún Laoghaire"}),</t>
+  </si>
+  <si>
+    <t>(DúnL: Constituency</t>
+  </si>
+  <si>
+    <t>(GE: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "GalwayEast"}),</t>
+  </si>
+  <si>
+    <t>(GW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Kerry"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Kildare North"}),</t>
+  </si>
+  <si>
+    <t>(KN: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Kildare South"}),</t>
+  </si>
+  <si>
+    <t>(KS: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Laois"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Limerick City"}),</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Limerick County"}),</t>
+  </si>
+  <si>
+    <t>(LC: Constituency</t>
+  </si>
+  <si>
+    <t>(LIM: Constituency</t>
+  </si>
+  <si>
+    <t>(LW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Louth"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Mayo"}),</t>
+  </si>
+  <si>
+    <t>(ME: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Meath East"}),</t>
+  </si>
+  <si>
+    <t>(MW: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Meath West"}),</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Offaly"}),</t>
+  </si>
+  <si>
+    <t>(OY: Constituency</t>
+  </si>
+  <si>
+    <t>(RG: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Sligo Leitrim"}),</t>
+  </si>
+  <si>
+    <t>Seats:"3", Name: "Roscommon Galway"}),</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Longford Westmeath"}),</t>
+  </si>
+  <si>
+    <t>(SL: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Tipperary"}),</t>
+  </si>
+  <si>
+    <t>(TIP: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Waterford"}),</t>
+  </si>
+  <si>
+    <t>(WTD: Constituency</t>
+  </si>
+  <si>
+    <t>(WXD: Constituency</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Wexford"}),</t>
+  </si>
+  <si>
+    <t>Seats:"5", Name: "Wicklow"}),</t>
+  </si>
+  <si>
+    <t>(WW: Constituency</t>
+  </si>
+  <si>
+    <t>(CK: Constituency</t>
+  </si>
+  <si>
+    <t>{Population: " 145,659",</t>
+  </si>
+  <si>
+    <t>{Population: " 120,483",</t>
+  </si>
+  <si>
+    <t>Seats:"4", Name: "Carlow-Kilkenny"}),</t>
   </si>
 </sst>
 </file>
@@ -612,17 +720,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection sqref="A1:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="2" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="6" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,46 +739,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>47</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,384 +786,395 @@
         <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted Constituency nodes and reentered them with interger values
</commit_message>
<xml_diff>
--- a/supports/Constituency.xlsx
+++ b/supports/Constituency.xlsx
@@ -74,24 +74,6 @@
     <t>{Population: "114660",</t>
   </si>
   <si>
-    <t>{Population: "144908",</t>
-  </si>
-  <si>
-    <t>{Population: "113179",</t>
-  </si>
-  <si>
-    <t>{Population: "118791",</t>
-  </si>
-  <si>
-    <t>{Population: "89564",</t>
-  </si>
-  <si>
-    <t>{Population: "150874",</t>
-  </si>
-  <si>
-    <t>{Population: "145502",</t>
-  </si>
-  <si>
     <t>{Population: "115350",</t>
   </si>
   <si>
@@ -267,9 +249,6 @@
     <t>Seats:"5", Name: "Dublin SouthWest"}),</t>
   </si>
   <si>
-    <t>Seats:"4", Name: "Dublin West"}),</t>
-  </si>
-  <si>
     <t>(DW: Constituency</t>
   </si>
   <si>
@@ -394,6 +373,27 @@
   </si>
   <si>
     <t>Seats:"4", Name: "Carlow-Kilkenny"}),</t>
+  </si>
+  <si>
+    <t>{Population = 144908,</t>
+  </si>
+  <si>
+    <t>{Population =113179,</t>
+  </si>
+  <si>
+    <t>Seats = 4, Name: "Dublin West"}),</t>
+  </si>
+  <si>
+    <t>{Population = 118791,</t>
+  </si>
+  <si>
+    <t>{Population = 89564,</t>
+  </si>
+  <si>
+    <t>{Population = 150874 ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Population = </t>
   </si>
 </sst>
 </file>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D41" sqref="B1:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,442 +739,442 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>